<commit_message>
Updated GHC7 map and waypoints
</commit_message>
<xml_diff>
--- a/XPlanningEvaluation/data/GHC7-waypoints.xlsx
+++ b/XPlanningEvaluation/data/GHC7-waypoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/XPlanningEvaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2794D71-E494-7247-8E3E-BBF063500D4D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A585918A-AA2C-ED41-9155-75437C2D12AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="560" windowWidth="21320" windowHeight="16560" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
+    <workbookView xWindow="12280" yWindow="560" windowWidth="21320" windowHeight="16560" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Location ID</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>24;25;28</t>
+  </si>
+  <si>
+    <t>15;20;23</t>
   </si>
 </sst>
 </file>
@@ -487,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A785292D-28EA-BB41-8A4F-1AF73CB8AC6A}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,8 +525,8 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1">
-        <v>0.2</v>
+      <c r="H1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -537,18 +540,18 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D2">
-        <f>B2+($H$1/2)</f>
+        <f>B2+($G$2/2)</f>
         <v>5.47</v>
       </c>
       <c r="E2">
-        <f>C2+($H$1/2)</f>
+        <f>C2+($G$2/2)</f>
         <v>1.1900000000000002</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
+      <c r="G2">
+        <v>0.2</v>
       </c>
       <c r="H2" s="1">
         <v>10</v>
@@ -565,11 +568,11 @@
         <v>0.98</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D33" si="0">B3+($H$1/2)</f>
+        <f>B3+($G$2/2)</f>
         <v>5.8</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E33" si="1">C3+($H$1/2)</f>
+        <f>C3+($G$2/2)</f>
         <v>1.08</v>
       </c>
       <c r="F3" t="s">
@@ -587,11 +590,11 @@
         <v>0.84</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>B4+($G$2/2)</f>
         <v>6.39</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f>C4+($G$2/2)</f>
         <v>0.94</v>
       </c>
       <c r="F4" t="s">
@@ -609,11 +612,11 @@
         <v>0.62</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>B5+($G$2/2)</f>
         <v>7.18</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f>C5+($G$2/2)</f>
         <v>0.72</v>
       </c>
       <c r="F5" t="s">
@@ -631,11 +634,11 @@
         <v>0.47</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>B6+($G$2/2)</f>
         <v>7.72</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f>C6+($G$2/2)</f>
         <v>0.56999999999999995</v>
       </c>
       <c r="F6" t="s">
@@ -653,11 +656,11 @@
         <v>1.55</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>B7+($G$2/2)</f>
         <v>5.17</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f>C7+($G$2/2)</f>
         <v>1.6500000000000001</v>
       </c>
       <c r="F7">
@@ -675,11 +678,11 @@
         <v>1.61</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>B8+($G$2/2)</f>
         <v>5.75</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f>C8+($G$2/2)</f>
         <v>1.7100000000000002</v>
       </c>
       <c r="F8" t="s">
@@ -697,11 +700,11 @@
         <v>1.65</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>B9+($G$2/2)</f>
         <v>6.33</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f>C9+($G$2/2)</f>
         <v>1.75</v>
       </c>
       <c r="F9" t="s">
@@ -719,11 +722,11 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>B10+($G$2/2)</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f>C10+($G$2/2)</f>
         <v>1.26</v>
       </c>
       <c r="F10" t="s">
@@ -741,11 +744,11 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>B11+($G$2/2)</f>
         <v>7.7799999999999994</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f>C11+($G$2/2)</f>
         <v>1.1900000000000002</v>
       </c>
       <c r="F11" t="s">
@@ -763,11 +766,11 @@
         <v>1.71</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f>B12+($G$2/2)</f>
         <v>7.1599999999999993</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f>C12+($G$2/2)</f>
         <v>1.81</v>
       </c>
       <c r="F12" t="s">
@@ -785,11 +788,11 @@
         <v>1.71</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>B13+($G$2/2)</f>
         <v>7.88</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f>C13+($G$2/2)</f>
         <v>1.81</v>
       </c>
       <c r="F13" t="s">
@@ -807,11 +810,11 @@
         <v>2.38</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>B14+($G$2/2)</f>
         <v>7.1199999999999992</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f>C14+($G$2/2)</f>
         <v>2.48</v>
       </c>
       <c r="F14" t="s">
@@ -829,11 +832,11 @@
         <v>3.18</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>B15+($G$2/2)</f>
         <v>5.3699999999999992</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f>C15+($G$2/2)</f>
         <v>3.2800000000000002</v>
       </c>
       <c r="F15">
@@ -851,11 +854,11 @@
         <v>3.18</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>B16+($G$2/2)</f>
         <v>5.8999999999999995</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f>C16+($G$2/2)</f>
         <v>3.2800000000000002</v>
       </c>
       <c r="F16" t="s">
@@ -873,11 +876,11 @@
         <v>3.18</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f>B17+($G$2/2)</f>
         <v>6.5299999999999994</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f>C17+($G$2/2)</f>
         <v>3.2800000000000002</v>
       </c>
       <c r="F17" t="s">
@@ -895,11 +898,11 @@
         <v>3.18</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>B18+($G$2/2)</f>
         <v>7.1199999999999992</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f>C18+($G$2/2)</f>
         <v>3.2800000000000002</v>
       </c>
       <c r="F18" t="s">
@@ -917,11 +920,11 @@
         <v>3.17</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>B19+($G$2/2)</f>
         <v>7.7299999999999995</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f>C19+($G$2/2)</f>
         <v>3.27</v>
       </c>
       <c r="F19" t="s">
@@ -939,15 +942,15 @@
         <v>3.77</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f>B20+($G$2/2)</f>
         <v>5.4899999999999993</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f>C20+($G$2/2)</f>
         <v>3.87</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -961,11 +964,11 @@
         <v>3.97</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>B21+($G$2/2)</f>
         <v>5.85</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f>C21+($G$2/2)</f>
         <v>4.07</v>
       </c>
       <c r="F21" t="s">
@@ -983,11 +986,11 @@
         <v>3.73</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>B22+($G$2/2)</f>
         <v>6.88</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f>C22+($G$2/2)</f>
         <v>3.83</v>
       </c>
       <c r="F22" t="s">
@@ -1005,11 +1008,11 @@
         <v>3.53</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>B23+($G$2/2)</f>
         <v>7.6199999999999992</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f>C23+($G$2/2)</f>
         <v>3.63</v>
       </c>
       <c r="F23" t="s">
@@ -1027,11 +1030,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f>B24+($G$2/2)</f>
         <v>5.75</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f>C24+($G$2/2)</f>
         <v>4.5</v>
       </c>
       <c r="F24" t="s">
@@ -1049,11 +1052,11 @@
         <v>4.5</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f>B25+($G$2/2)</f>
         <v>6.1499999999999995</v>
       </c>
       <c r="E25">
-        <f>C25+($H$1/2)</f>
+        <f>C25+($G$2/2)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="F25" t="s">
@@ -1071,11 +1074,11 @@
         <v>4.17</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f>B26+($G$2/2)</f>
         <v>6.85</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f>C26+($G$2/2)</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="F26" t="s">
@@ -1093,11 +1096,11 @@
         <v>4.07</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f>B27+($G$2/2)</f>
         <v>7.46</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f>C27+($G$2/2)</f>
         <v>4.17</v>
       </c>
       <c r="F27" t="s">
@@ -1115,11 +1118,11 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f>B28+($G$2/2)</f>
         <v>6.68</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
+        <f>C28+($G$2/2)</f>
         <v>4.6599999999999993</v>
       </c>
       <c r="F28" t="s">
@@ -1137,11 +1140,11 @@
         <v>5.34</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f>B29+($G$2/2)</f>
         <v>6.43</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f>C29+($G$2/2)</f>
         <v>5.4399999999999995</v>
       </c>
       <c r="F29" t="s">
@@ -1159,11 +1162,11 @@
         <v>5.8</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f>B30+($G$2/2)</f>
         <v>6.4099999999999993</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f>C30+($G$2/2)</f>
         <v>5.8999999999999995</v>
       </c>
       <c r="F30" t="s">
@@ -1181,11 +1184,11 @@
         <v>6.41</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f>B31+($G$2/2)</f>
         <v>6.39</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
+        <f>C31+($G$2/2)</f>
         <v>6.51</v>
       </c>
       <c r="F31">
@@ -1203,11 +1206,11 @@
         <v>5.98</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f>B32+($G$2/2)</f>
         <v>6.9499999999999993</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f>C32+($G$2/2)</f>
         <v>6.08</v>
       </c>
       <c r="F32" t="s">
@@ -1225,11 +1228,11 @@
         <v>6.17</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f>B33+($G$2/2)</f>
         <v>7.46</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
+        <f>C33+($G$2/2)</f>
         <v>6.27</v>
       </c>
       <c r="F33">

</xml_diff>

<commit_message>
Fixed edge-asymmetry in GHC7-waypoints
</commit_message>
<xml_diff>
--- a/XPlanningEvaluation/data/GHC7-waypoints.xlsx
+++ b/XPlanningEvaluation/data/GHC7-waypoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/XPlanningEvaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A585918A-AA2C-ED41-9155-75437C2D12AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F30023A-6681-514A-893B-ADC6E92D2790}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="560" windowWidth="21320" windowHeight="16560" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
+    <workbookView xWindow="2100" yWindow="2160" windowWidth="21320" windowHeight="16560" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>17;22</t>
   </si>
   <si>
-    <t>15;23</t>
-  </si>
-  <si>
     <t>17;25</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>15;20;23</t>
+  </si>
+  <si>
+    <t>15;19;23</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,11 +540,11 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D2">
-        <f>B2+($G$2/2)</f>
+        <f t="shared" ref="D2:D33" si="0">B2+($G$2/2)</f>
         <v>5.47</v>
       </c>
       <c r="E2">
-        <f>C2+($G$2/2)</f>
+        <f t="shared" ref="E2:E33" si="1">C2+($G$2/2)</f>
         <v>1.1900000000000002</v>
       </c>
       <c r="F2">
@@ -568,11 +568,11 @@
         <v>0.98</v>
       </c>
       <c r="D3">
-        <f>B3+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
       <c r="E3">
-        <f>C3+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.08</v>
       </c>
       <c r="F3" t="s">
@@ -590,11 +590,11 @@
         <v>0.84</v>
       </c>
       <c r="D4">
-        <f>B4+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.39</v>
       </c>
       <c r="E4">
-        <f>C4+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>0.94</v>
       </c>
       <c r="F4" t="s">
@@ -612,11 +612,11 @@
         <v>0.62</v>
       </c>
       <c r="D5">
-        <f>B5+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.18</v>
       </c>
       <c r="E5">
-        <f>C5+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
       <c r="F5" t="s">
@@ -634,11 +634,11 @@
         <v>0.47</v>
       </c>
       <c r="D6">
-        <f>B6+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.72</v>
       </c>
       <c r="E6">
-        <f>C6+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>0.56999999999999995</v>
       </c>
       <c r="F6" t="s">
@@ -656,11 +656,11 @@
         <v>1.55</v>
       </c>
       <c r="D7">
-        <f>B7+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.17</v>
       </c>
       <c r="E7">
-        <f>C7+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.6500000000000001</v>
       </c>
       <c r="F7">
@@ -678,11 +678,11 @@
         <v>1.61</v>
       </c>
       <c r="D8">
-        <f>B8+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.75</v>
       </c>
       <c r="E8">
-        <f>C8+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.7100000000000002</v>
       </c>
       <c r="F8" t="s">
@@ -700,11 +700,11 @@
         <v>1.65</v>
       </c>
       <c r="D9">
-        <f>B9+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.33</v>
       </c>
       <c r="E9">
-        <f>C9+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
       <c r="F9" t="s">
@@ -722,11 +722,11 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D10">
-        <f>B10+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.1499999999999995</v>
       </c>
       <c r="E10">
-        <f>C10+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
       <c r="F10" t="s">
@@ -744,11 +744,11 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D11">
-        <f>B11+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.7799999999999994</v>
       </c>
       <c r="E11">
-        <f>C11+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.1900000000000002</v>
       </c>
       <c r="F11" t="s">
@@ -766,11 +766,11 @@
         <v>1.71</v>
       </c>
       <c r="D12">
-        <f>B12+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.1599999999999993</v>
       </c>
       <c r="E12">
-        <f>C12+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.81</v>
       </c>
       <c r="F12" t="s">
@@ -788,11 +788,11 @@
         <v>1.71</v>
       </c>
       <c r="D13">
-        <f>B13+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.88</v>
       </c>
       <c r="E13">
-        <f>C13+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>1.81</v>
       </c>
       <c r="F13" t="s">
@@ -810,11 +810,11 @@
         <v>2.38</v>
       </c>
       <c r="D14">
-        <f>B14+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.1199999999999992</v>
       </c>
       <c r="E14">
-        <f>C14+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>2.48</v>
       </c>
       <c r="F14" t="s">
@@ -832,11 +832,11 @@
         <v>3.18</v>
       </c>
       <c r="D15">
-        <f>B15+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.3699999999999992</v>
       </c>
       <c r="E15">
-        <f>C15+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
       <c r="F15">
@@ -854,11 +854,11 @@
         <v>3.18</v>
       </c>
       <c r="D16">
-        <f>B16+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.8999999999999995</v>
       </c>
       <c r="E16">
-        <f>C16+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
       <c r="F16" t="s">
@@ -876,11 +876,11 @@
         <v>3.18</v>
       </c>
       <c r="D17">
-        <f>B17+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.5299999999999994</v>
       </c>
       <c r="E17">
-        <f>C17+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
       <c r="F17" t="s">
@@ -898,11 +898,11 @@
         <v>3.18</v>
       </c>
       <c r="D18">
-        <f>B18+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.1199999999999992</v>
       </c>
       <c r="E18">
-        <f>C18+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
       <c r="F18" t="s">
@@ -920,11 +920,11 @@
         <v>3.17</v>
       </c>
       <c r="D19">
-        <f>B19+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.7299999999999995</v>
       </c>
       <c r="E19">
-        <f>C19+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.27</v>
       </c>
       <c r="F19" t="s">
@@ -942,15 +942,15 @@
         <v>3.77</v>
       </c>
       <c r="D20">
-        <f>B20+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.4899999999999993</v>
       </c>
       <c r="E20">
-        <f>C20+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.87</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -964,15 +964,15 @@
         <v>3.97</v>
       </c>
       <c r="D21">
-        <f>B21+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.85</v>
       </c>
       <c r="E21">
-        <f>C21+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>4.07</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -986,15 +986,15 @@
         <v>3.73</v>
       </c>
       <c r="D22">
-        <f>B22+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.88</v>
       </c>
       <c r="E22">
-        <f>C22+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.83</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1008,15 +1008,15 @@
         <v>3.53</v>
       </c>
       <c r="D23">
-        <f>B23+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.6199999999999992</v>
       </c>
       <c r="E23">
-        <f>C23+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>3.63</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1030,15 +1030,15 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D24">
-        <f>B24+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>5.75</v>
       </c>
       <c r="E24">
-        <f>C24+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1052,15 +1052,15 @@
         <v>4.5</v>
       </c>
       <c r="D25">
-        <f>B25+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.1499999999999995</v>
       </c>
       <c r="E25">
-        <f>C25+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1074,15 +1074,15 @@
         <v>4.17</v>
       </c>
       <c r="D26">
-        <f>B26+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.85</v>
       </c>
       <c r="E26">
-        <f>C26+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>4.2699999999999996</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1096,15 +1096,15 @@
         <v>4.07</v>
       </c>
       <c r="D27">
-        <f>B27+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.46</v>
       </c>
       <c r="E27">
-        <f>C27+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>4.17</v>
       </c>
       <c r="F27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1118,15 +1118,15 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="D28">
-        <f>B28+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.68</v>
       </c>
       <c r="E28">
-        <f>C28+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>4.6599999999999993</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1140,15 +1140,15 @@
         <v>5.34</v>
       </c>
       <c r="D29">
-        <f>B29+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.43</v>
       </c>
       <c r="E29">
-        <f>C29+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>5.4399999999999995</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1162,15 +1162,15 @@
         <v>5.8</v>
       </c>
       <c r="D30">
-        <f>B30+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.4099999999999993</v>
       </c>
       <c r="E30">
-        <f>C30+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>5.8999999999999995</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1184,11 +1184,11 @@
         <v>6.41</v>
       </c>
       <c r="D31">
-        <f>B31+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.39</v>
       </c>
       <c r="E31">
-        <f>C31+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>6.51</v>
       </c>
       <c r="F31">
@@ -1206,15 +1206,15 @@
         <v>5.98</v>
       </c>
       <c r="D32">
-        <f>B32+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>6.9499999999999993</v>
       </c>
       <c r="E32">
-        <f>C32+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>6.08</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1228,11 +1228,11 @@
         <v>6.17</v>
       </c>
       <c r="D33">
-        <f>B33+($G$2/2)</f>
+        <f t="shared" si="0"/>
         <v>7.46</v>
       </c>
       <c r="E33">
-        <f>C33+($G$2/2)</f>
+        <f t="shared" si="1"/>
         <v>6.27</v>
       </c>
       <c r="F33">

</xml_diff>

<commit_message>
Added additional way-points X1-5 to GHC7-map.pptx and GHC7-waypoints.xlsx
</commit_message>
<xml_diff>
--- a/XPlanningEvaluation/data/GHC7-waypoints.xlsx
+++ b/XPlanningEvaluation/data/GHC7-waypoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/XPlanningEvaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F30023A-6681-514A-893B-ADC6E92D2790}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17CF53F-5D81-FD4E-B1B1-455F31E31138}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="2160" windowWidth="21320" windowHeight="16560" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
+    <workbookView xWindow="38440" yWindow="460" windowWidth="30580" windowHeight="19960" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Location ID</t>
   </si>
@@ -136,6 +136,36 @@
   </si>
   <si>
     <t>15;19;23</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>6;14</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>8;16</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>12;18</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>23;29</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>26;31</t>
   </si>
 </sst>
 </file>
@@ -488,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A785292D-28EA-BB41-8A4F-1AF73CB8AC6A}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,11 +570,11 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D33" si="0">B2+($G$2/2)</f>
+        <f t="shared" ref="D2:D38" si="0">B2+($G$2/2)</f>
         <v>5.47</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E33" si="1">C2+($G$2/2)</f>
+        <f t="shared" ref="E2:E38" si="1">C2+($G$2/2)</f>
         <v>1.1900000000000002</v>
       </c>
       <c r="F2">
@@ -1237,6 +1267,116 @@
       </c>
       <c r="F33">
         <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>5.17</v>
+      </c>
+      <c r="C34">
+        <v>2.38</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>5.27</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>6.35</v>
+      </c>
+      <c r="C35">
+        <v>2.38</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>6.4499999999999993</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>7.72</v>
+      </c>
+      <c r="C36">
+        <v>2.38</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>7.8199999999999994</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <v>5.68</v>
+      </c>
+      <c r="C37">
+        <v>5.55</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>5.7799999999999994</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>5.6499999999999995</v>
+      </c>
+      <c r="F37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38">
+        <v>7.04</v>
+      </c>
+      <c r="C38">
+        <v>5.23</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>7.14</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>5.33</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GHC7-waypoints: symmetric connections between nodes
</commit_message>
<xml_diff>
--- a/XPlanningEvaluation/data/GHC7-waypoints.xlsx
+++ b/XPlanningEvaluation/data/GHC7-waypoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/XPlanningEvaluation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17CF53F-5D81-FD4E-B1B1-455F31E31138}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743810FC-86D3-A748-A223-76202412F3CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38440" yWindow="460" windowWidth="30580" windowHeight="19960" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
+    <workbookView xWindow="4400" yWindow="1340" windowWidth="30580" windowHeight="19960" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Location ID</t>
   </si>
@@ -72,9 +72,6 @@
     <t>2;6;8</t>
   </si>
   <si>
-    <t>7;11</t>
-  </si>
-  <si>
     <t>4;11</t>
   </si>
   <si>
@@ -84,51 +81,30 @@
     <t>8;9;12;13</t>
   </si>
   <si>
-    <t>10;11</t>
-  </si>
-  <si>
     <t>11;17</t>
   </si>
   <si>
     <t>14;16;19;20</t>
   </si>
   <si>
-    <t>15;17</t>
-  </si>
-  <si>
     <t>13;16;18;21</t>
   </si>
   <si>
-    <t>17;22</t>
-  </si>
-  <si>
     <t>17;25</t>
   </si>
   <si>
     <t>18;26</t>
   </si>
   <si>
-    <t>19;20;24</t>
-  </si>
-  <si>
     <t>23;27</t>
   </si>
   <si>
     <t>21;26;27</t>
   </si>
   <si>
-    <t>22;25</t>
-  </si>
-  <si>
     <t>27;29</t>
   </si>
   <si>
-    <t>28;30;31</t>
-  </si>
-  <si>
-    <t>29;32</t>
-  </si>
-  <si>
     <t>24;25;28</t>
   </si>
   <si>
@@ -166,6 +142,36 @@
   </si>
   <si>
     <t>26;31</t>
+  </si>
+  <si>
+    <t>7;X1</t>
+  </si>
+  <si>
+    <t>15;X1</t>
+  </si>
+  <si>
+    <t>7;11;X2</t>
+  </si>
+  <si>
+    <t>15;17;X2</t>
+  </si>
+  <si>
+    <t>10;11;X3</t>
+  </si>
+  <si>
+    <t>17;22;X3</t>
+  </si>
+  <si>
+    <t>19;20;24;X4</t>
+  </si>
+  <si>
+    <t>28;30;31;X4</t>
+  </si>
+  <si>
+    <t>22;25;X5</t>
+  </si>
+  <si>
+    <t>29;32;X5</t>
   </si>
 </sst>
 </file>
@@ -521,7 +527,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,8 +699,8 @@
         <f t="shared" si="1"/>
         <v>1.6500000000000001</v>
       </c>
-      <c r="F7">
-        <v>7</v>
+      <c r="F7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -738,7 +744,7 @@
         <v>1.75</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -760,7 +766,7 @@
         <v>1.26</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -782,7 +788,7 @@
         <v>1.1900000000000002</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -804,7 +810,7 @@
         <v>1.81</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -826,7 +832,7 @@
         <v>1.81</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -848,7 +854,7 @@
         <v>2.48</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -869,8 +875,8 @@
         <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
-      <c r="F15">
-        <v>15</v>
+      <c r="F15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -892,7 +898,7 @@
         <v>3.2800000000000002</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -914,7 +920,7 @@
         <v>3.2800000000000002</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -936,7 +942,7 @@
         <v>3.2800000000000002</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -958,7 +964,7 @@
         <v>3.27</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -980,7 +986,7 @@
         <v>3.87</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1002,7 +1008,7 @@
         <v>4.07</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1024,7 +1030,7 @@
         <v>3.83</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1046,7 +1052,7 @@
         <v>3.63</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1068,7 +1074,7 @@
         <v>4.5</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1090,7 +1096,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1112,7 +1118,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1134,7 +1140,7 @@
         <v>4.17</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1156,7 +1162,7 @@
         <v>4.6599999999999993</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1178,7 +1184,7 @@
         <v>5.4399999999999995</v>
       </c>
       <c r="F29" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1200,7 +1206,7 @@
         <v>5.8999999999999995</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1244,7 +1250,7 @@
         <v>6.08</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1271,7 +1277,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B34">
         <v>5.17</v>
@@ -1288,12 +1294,12 @@
         <v>2.48</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B35">
         <v>6.35</v>
@@ -1310,12 +1316,12 @@
         <v>2.48</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B36">
         <v>7.72</v>
@@ -1332,12 +1338,12 @@
         <v>2.48</v>
       </c>
       <c r="F36" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B37">
         <v>5.68</v>
@@ -1354,12 +1360,12 @@
         <v>5.6499999999999995</v>
       </c>
       <c r="F37" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>7.04</v>
@@ -1376,7 +1382,7 @@
         <v>5.33</v>
       </c>
       <c r="F38" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>